<commit_message>
Tasks assignment summary for all members. (Kaii)
</commit_message>
<xml_diff>
--- a/PCB/06 Requirement Management/Product Backlog_V0.2_20150911.xlsx
+++ b/PCB/06 Requirement Management/Product Backlog_V0.2_20150911.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="40" windowWidth="25420" windowHeight="13480" tabRatio="500"/>
+    <workbookView xWindow="15" yWindow="105" windowWidth="25425" windowHeight="13425" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Produc Backlog" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Produc Backlog'!$1:$3</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -245,6 +245,62 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t xml:space="preserve">1. Visitor will register or login at last point, before payment.
+2. All the success stories will be provided by categories.
+3. User categories as
+     - Student
+     - Migrant
+     - Worker who want to change career
+     - Jobless
+     - Kiwi
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Statics pages, and should be mobile friendly.
+2. Detail information on current PHP system can be reused.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Visitor will register or login at last point, before payment.
+2. In detail page of success story, courses should be list and can be check to make order.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.NET MVC5
+bootstrap
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.NET MVC5
+bootstrap
+MySQL
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11. A demo with set of web pages with mobile friendly layout to show the purchasing process of visitors or un-login students.
+2. A shopping basket with demo pages.
+3. A demo page includes:
+   - Survey pages
+   - Success stories page
+   - Shopping basket page
+   - Purchasing confirm page
+4. A survey design for individual visitor, client company and registered student.
+5. A set of new table(s) to store the data of success stories.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a visitor (anonymous)
+I would like to read the detail of  some success story.
+So that I can order the same courses.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">As a visitor (anonymous user)
+I would like to read some success stories of previous students.
+So that I can follow the same approach.
+</t>
+  </si>
+  <si>
     <r>
       <t>As CEO,
 I would like to re-design our website(</t>
@@ -268,67 +324,10 @@
 So that we can meet ranking requirement, because Google adopted mobile-friendliness as a ranking signal.
 </t>
     </r>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Visitor will register or login at last point, before payment.
-2. All the success stories will be provided by categories.
-3. User categories as
-     - Student
-     - Migrant
-     - Worker who want to change career
-     - Jobless
-     - Kiwi
-</t>
   </si>
   <si>
     <t xml:space="preserve">As CEO
-I would like out team profile and FAQ to be well noticed. So that we can provide more detail information about our company. 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Statics pages, and should be mobile friendly.
-2. Detail information on current PHP system can be reused.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. Visitor will register or login at last point, before payment.
-2. In detail page of success story, courses should be list and can be check to make order.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.NET MVC5
-bootstrap
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">.NET MVC5
-bootstrap
-MySQL
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11. A demo with set of web pages with mobile friendly layout to show the purchasing process of visitors or un-login students.
-2. A shopping basket with demo pages.
-3. A demo page includes:
-   - Survey pages
-   - Success stories page
-   - Shopping basket page
-   - Purchasing confirm page
-4. A survey design for individual visitor, client company and registered student.
-5. A set of new table(s) to store the data of success stories.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a visitor (anonymous)
-I would like to read the detail of  some success story.
-So that I can order the same courses.
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">As a visitor (anonymous user)
-I would like to read some success stories of previous students.
-So that I can follow the same approach.
+I would like our team profile and FAQ to be well noticed. So that we can provide more detail information about our company. 
 </t>
   </si>
 </sst>
@@ -336,7 +335,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -669,6 +668,15 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -684,19 +692,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -829,6 +828,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1158,38 +1162,38 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="2.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="2.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5" style="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="50.6640625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="56.6640625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="41.83203125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.83203125" style="7" customWidth="1"/>
-    <col min="7" max="16384" width="2.83203125" style="7"/>
+    <col min="3" max="3" width="50.625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="56.625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="41.875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.875" style="7" customWidth="1"/>
+    <col min="7" max="16384" width="2.875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="18">
+    <row r="1" spans="1:6" ht="20.25">
       <c r="A1" s="13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="17" customHeight="1">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:6" ht="17.100000000000001" customHeight="1">
+      <c r="A2" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="17"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="14" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" s="6" customFormat="1" ht="17" customHeight="1">
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" spans="1:6" s="6" customFormat="1" ht="17.100000000000001" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1210,96 +1214,96 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="120">
-      <c r="A4" s="20">
+      <c r="A4" s="14">
         <v>1</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="14">
         <v>1</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="D4" s="21" t="s">
+      <c r="C4" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="22" t="s">
-        <v>39</v>
+      <c r="F4" s="16" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="90" customHeight="1">
-      <c r="A5" s="20">
+      <c r="A5" s="14">
         <f>A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="14">
         <v>2</v>
       </c>
-      <c r="C5" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="E5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="F5" s="23" t="s">
-        <v>40</v>
+      <c r="D5" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="60">
-      <c r="A6" s="20">
+      <c r="A6" s="14">
         <f>A5+1</f>
         <v>3</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B6" s="14">
         <v>2</v>
       </c>
-      <c r="C6" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="23"/>
-      <c r="F6" s="23"/>
+      <c r="C6" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
     </row>
     <row r="7" spans="1:6" ht="75">
-      <c r="A7" s="20">
+      <c r="A7" s="14">
         <f>A6+1</f>
         <v>4</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="14">
         <v>1</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-    </row>
-    <row r="8" spans="1:6" ht="80" customHeight="1">
-      <c r="A8" s="20">
-        <f t="shared" ref="A6:A14" si="0">A7+1</f>
+      <c r="C7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+    </row>
+    <row r="8" spans="1:6" ht="80.099999999999994" customHeight="1">
+      <c r="A8" s="14">
+        <f t="shared" ref="A8:A14" si="0">A7+1</f>
         <v>5</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B8" s="14">
         <v>2</v>
       </c>
-      <c r="C8" s="21" t="s">
+      <c r="C8" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
     </row>
     <row r="9" spans="1:6" ht="90">
       <c r="A9" s="4">
@@ -1320,7 +1324,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="135">
+    <row r="10" spans="1:6" ht="120">
       <c r="A10" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1389,10 +1393,10 @@
       <c r="D13" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="19" t="s">
+      <c r="F13" s="23" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1408,8 +1412,8 @@
       <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="19"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="4"/>

</xml_diff>